<commit_message>
feat(depths): calculate depths for all return periods-JIRA-918
</commit_message>
<xml_diff>
--- a/Lookuptables/AAL.xlsx
+++ b/Lookuptables/AAL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\nhrap-dev\FAST\Lookuptables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\test\FAST\Lookuptables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CE783F-A332-4EF2-AB02-E0C6D5B6EEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB6C753-8A6C-4243-9DFF-CC60FF53EBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C3D9F35B-9A87-4C41-8185-A06FC2E6597C}"/>
+    <workbookView xWindow="1440" yWindow="1188" windowWidth="21600" windowHeight="11328" xr2:uid="{C3D9F35B-9A87-4C41-8185-A06FC2E6597C}"/>
   </bookViews>
   <sheets>
     <sheet name="A Zones" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
   <si>
     <t>A01</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Check points 0.2%</t>
+  </si>
+  <si>
+    <t>PELV_50</t>
   </si>
 </sst>
 </file>
@@ -197,13 +200,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,7 +528,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="E2" sqref="C2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -587,31 +594,34 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="B2" s="1">
         <v>1000</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="7">
         <v>500</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="7">
         <v>250</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="7">
         <v>200</v>
       </c>
       <c r="F2" s="4">
         <v>100</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="7">
         <v>75</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="7">
         <v>50</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="7">
         <v>25</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="7">
         <v>10</v>
       </c>
       <c r="K2" s="1"/>
@@ -2329,5 +2339,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>